<commit_message>
Excel sheet reader and card details excel sheet update, fill card details page completed
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/cardDetails.xlsx
+++ b/src/main/resources/Data/cardDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndhurandher\intellij-workspace\hu-selenium-assignment-ag\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B41AF-F4C8-4525-B48D-01180E11CA79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406F4B1D-E0F7-4A3A-809E-D520D9428153}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,13 +54,13 @@
     <t>abc3@gmail.com</t>
   </si>
   <si>
-    <t>"4242424242424240"</t>
-  </si>
-  <si>
-    <t>"5555555555554440"</t>
-  </si>
-  <si>
-    <t>"4000056655665550"</t>
+    <t>"4242424242424242"</t>
+  </si>
+  <si>
+    <t>"4000056655665556"</t>
+  </si>
+  <si>
+    <t>"5555555555554444"</t>
   </si>
 </sst>
 </file>

</xml_diff>